<commit_message>
Added 1x8 header to BOM.
</commit_message>
<xml_diff>
--- a/src/1.0/BOM.xlsx
+++ b/src/1.0/BOM.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12315" windowHeight="5130"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="22180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>Part</t>
   </si>
@@ -129,9 +134,6 @@
     <t>1X08_SQ1</t>
   </si>
   <si>
-    <t>1x8 Headers</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
@@ -208,13 +210,31 @@
   </si>
   <si>
     <t>FB1,FB2</t>
+  </si>
+  <si>
+    <t>609-3273-ND</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>68001-108HLF</t>
+  </si>
+  <si>
+    <t>1x8</t>
+  </si>
+  <si>
+    <t>1x8 Headers Gold 30uin</t>
+  </si>
+  <si>
+    <t>0.230in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +245,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -247,8 +283,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -262,7 +322,31 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="25">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,22 +638,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -609,7 +693,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -638,7 +722,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
@@ -667,7 +751,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>25</v>
@@ -690,7 +774,7 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
@@ -723,122 +807,147 @@
         <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="28">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>